<commit_message>
New code for checking ISR
</commit_message>
<xml_diff>
--- a/Backlog/Tasks.xlsx
+++ b/Backlog/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\all\Important\praca\kafka\kafka_montool\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA6A227-EAB2-4F8F-8DFF-726DB2199F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48466370-57E3-48E7-9A36-6D78D30C13D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20388" yWindow="7752" windowWidth="17280" windowHeight="8928" xr2:uid="{47695776-9741-4823-B87E-216679646C64}"/>
+    <workbookView xWindow="-23148" yWindow="4992" windowWidth="23256" windowHeight="12456" xr2:uid="{47695776-9741-4823-B87E-216679646C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Kafka Lag &amp; Health Monitoring Platform</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Spring Boot skeleton</t>
-  </si>
-  <si>
-    <t>Konfiguracja lokalna + profile</t>
   </si>
   <si>
     <t>🎯 EPIC 2: Kafka Cluster Health</t>
@@ -271,7 +268,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -609,7 +608,7 @@
   <dimension ref="A1:B90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -634,63 +633,58 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18">
       <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -698,32 +692,32 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18">
       <c r="A24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -731,7 +725,7 @@
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:1">
@@ -739,7 +733,7 @@
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:1">
@@ -747,7 +741,7 @@
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:1">
@@ -755,27 +749,27 @@
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="18">
       <c r="A44" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:1">
@@ -783,22 +777,22 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="18">
       <c r="A56" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:1">
@@ -806,7 +800,7 @@
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:1">
@@ -814,7 +808,7 @@
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:1">
@@ -822,7 +816,7 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:1">
@@ -830,22 +824,22 @@
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="18">
       <c r="A72" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:1">
@@ -853,32 +847,32 @@
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="18">
       <c r="A82" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Consumer listing first try
</commit_message>
<xml_diff>
--- a/Backlog/Tasks.xlsx
+++ b/Backlog/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\all\Important\praca\kafka\kafka_montool\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BFBDD4-B1BB-430C-838A-70DA5977E857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D7676D-294D-4C5F-BCC0-68BA57C873F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{47695776-9741-4823-B87E-216679646C64}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15285" xr2:uid="{47695776-9741-4823-B87E-216679646C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -269,6 +269,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -607,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21F580A-CB07-4624-88FC-BE256E302E58}">
   <dimension ref="A1:A45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -687,7 +690,7 @@
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>